<commit_message>
added a tab for placeholders
</commit_message>
<xml_diff>
--- a/reporting_filter_frames/filter_frames.xlsx
+++ b/reporting_filter_frames/filter_frames.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings-demo\reporting_filter_frames\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Desktop\reporting_filter_frames\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AD3463-A0EA-41AF-A942-3D69A2BBBE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8123DF4-D6C4-4375-97E7-BE3820A53F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{4619326B-ED9C-4FC6-93BB-2E68FB3C5980}"/>
   </bookViews>
   <sheets>
-    <sheet name="Filters" sheetId="1" r:id="rId1"/>
-    <sheet name="Frames" sheetId="22" r:id="rId2"/>
+    <sheet name="Placeholder" sheetId="23" r:id="rId1"/>
+    <sheet name="Filters" sheetId="1" r:id="rId2"/>
+    <sheet name="Frames" sheetId="22" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -73,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>{{ holdings }}</t>
   </si>
@@ -112,6 +113,9 @@
   </si>
   <si>
     <t>{{ holdings | head(3) | columns(0, 4) }}</t>
+  </si>
+  <si>
+    <t>Full Table</t>
   </si>
 </sst>
 </file>
@@ -121,7 +125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,14 +142,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -153,6 +149,19 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Gill Sans MT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Gill Sans MT"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Gill Sans MT"/>
       <family val="2"/>
@@ -185,29 +194,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Gill Sans MT"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Gill Sans MT"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -216,6 +253,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
+        <color theme="1"/>
         <name val="Gill Sans MT"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -231,11 +269,38 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
+        <color theme="1"/>
         <name val="Gill Sans MT"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Gill Sans MT"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Gill Sans MT"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -245,6 +310,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
+        <color theme="1"/>
         <name val="Gill Sans MT"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -260,6 +326,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
+        <color theme="1"/>
         <name val="Gill Sans MT"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -274,12 +341,25 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
+        <color theme="1"/>
         <name val="Gill Sans MT"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Gill Sans MT"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -289,10 +369,12 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
+        <color theme="1"/>
         <name val="Gill Sans MT"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -303,6 +385,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
+        <color theme="1"/>
         <name val="Gill Sans MT"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -389,13 +472,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="TableStyleXlwings" pivot="0" count="7" xr9:uid="{41E744D9-6FB5-496B-B189-66108412DCA5}">
-      <tableStyleElement type="wholeTable" dxfId="13"/>
-      <tableStyleElement type="headerRow" dxfId="12"/>
-      <tableStyleElement type="totalRow" dxfId="11"/>
-      <tableStyleElement type="firstColumn" dxfId="10"/>
-      <tableStyleElement type="lastColumn" dxfId="9"/>
-      <tableStyleElement type="firstRowStripe" dxfId="8"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="7"/>
+      <tableStyleElement type="wholeTable" dxfId="18"/>
+      <tableStyleElement type="headerRow" dxfId="17"/>
+      <tableStyleElement type="totalRow" dxfId="16"/>
+      <tableStyleElement type="firstColumn" dxfId="15"/>
+      <tableStyleElement type="lastColumn" dxfId="14"/>
+      <tableStyleElement type="firstRowStripe" dxfId="13"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="12"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -410,42 +493,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{6D68FD5D-3D0A-4CDD-9FD3-F24769B81F97}" name="Table7" displayName="Table7" ref="A3:B4" totalsRowShown="0" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{6D68FD5D-3D0A-4CDD-9FD3-F24769B81F97}" name="Table7" displayName="Table7" ref="A3:B4" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A3:B4" xr:uid="{6D68FD5D-3D0A-4CDD-9FD3-F24769B81F97}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{296AC5B1-7110-440D-847A-B8A9D9F6FB7F}" name="{{ holdings | head(10) | columns(0, 4) }}" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{03278D61-BCE0-4408-AA4D-56E7402423E4}" name=" " dataDxfId="4" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{296AC5B1-7110-440D-847A-B8A9D9F6FB7F}" name="{{ holdings | head(10) | columns(0, 4) }}" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{03278D61-BCE0-4408-AA4D-56E7402423E4}" name=" " dataDxfId="10" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleXlwings" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{D2ABDDA3-3204-4329-8B7D-813D882CDA11}" name="Table728" displayName="Table728" ref="D3:E4" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{D2ABDDA3-3204-4329-8B7D-813D882CDA11}" name="Table728" displayName="Table728" ref="D3:E4" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="D3:E4" xr:uid="{D2ABDDA3-3204-4329-8B7D-813D882CDA11}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E340CCC9-929E-4233-821D-5E8DD3B6EA8C}" name="{{ holdings | head(5) | columns(0, 4) }}" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{1016760A-9DCD-4EC5-9E4A-51C4B0D473E2}" name=" " dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{E340CCC9-929E-4233-821D-5E8DD3B6EA8C}" name="{{ holdings | head(5) | columns(0, 4) }}" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{1016760A-9DCD-4EC5-9E4A-51C4B0D473E2}" name=" " dataDxfId="6" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleXlwings" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{75B6FE59-6C4E-4B67-8500-B06B2496EE1A}" name="Table72839" displayName="Table72839" ref="D6:E7" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{75B6FE59-6C4E-4B67-8500-B06B2496EE1A}" name="Table72839" displayName="Table72839" ref="D6:E7" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
   <autoFilter ref="D6:E7" xr:uid="{75B6FE59-6C4E-4B67-8500-B06B2496EE1A}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{49C845BC-4039-4D59-8A43-FF47E8848386}" name="{{ holdings | head(3) | columns(0, 4) }}" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{4B967A61-119D-4E9C-9BEB-BA2ACD0B95A2}" name=" " dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{49C845BC-4039-4D59-8A43-FF47E8848386}" name="{{ holdings | head(3) | columns(0, 4) }}" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{4B967A61-119D-4E9C-9BEB-BA2ACD0B95A2}" name=" " dataDxfId="2" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleXlwings" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -747,151 +830,293 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B269E39-E957-4FB8-9214-2252A7C1360C}">
-  <dimension ref="A1:Q31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE74CF58-CEAE-4820-B656-2FDEF93B1CD8}">
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="21.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.53125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.06640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="6"/>
-      <c r="G1" s="1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E31" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B269E39-E957-4FB8-9214-2252A7C1360C}">
+  <dimension ref="A1:Q38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.6"/>
+  <cols>
+    <col min="1" max="1" width="21.53125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="9.06640625" style="5"/>
+    <col min="7" max="7" width="16.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="9.06640625" style="5"/>
+    <col min="13" max="13" width="20.796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.06640625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="A1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E3" s="7"/>
-      <c r="G3" s="2" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="9"/>
+      <c r="G3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="6"/>
-      <c r="M3" s="2" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="9"/>
+      <c r="M3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="6"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="Q4" s="7"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="Q5" s="7"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="Q6" s="7"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="Q7" s="7"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="Q8" s="7"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E27" s="7"/>
-    </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.45">
-      <c r="E31" s="7"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="9"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="E4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="Q4" s="6"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="E5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="Q5" s="6"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="E6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="Q6" s="6"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="E7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="Q7" s="6"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="E8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="Q8" s="6"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.6">
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.6">
+      <c r="E38" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -899,80 +1124,82 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAC22E9-B08C-4D82-8667-ECFF551F8508}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.149999999999999" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="32.265625" customWidth="1"/>
-    <col min="2" max="2" width="15.73046875" customWidth="1"/>
-    <col min="4" max="4" width="32.265625" customWidth="1"/>
-    <col min="5" max="5" width="15.73046875" customWidth="1"/>
+    <col min="1" max="1" width="32.265625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="15.73046875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.06640625" style="5"/>
+    <col min="4" max="4" width="32.265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.73046875" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="9.06640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="D6" t="s">
+      <c r="B6" s="1"/>
+      <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="D9" s="3" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.6">
+      <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>